<commit_message>
Alg - Formatting and clean-up
</commit_message>
<xml_diff>
--- a/Algoritmia/tables/lab3/all.xlsx
+++ b/Algoritmia/tables/lab3/all.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="insertion" sheetId="1" r:id="rId1"/>
-    <sheet name="bubble" sheetId="2" r:id="rId2"/>
+    <sheet name="bubble" sheetId="2" r:id="rId1"/>
+    <sheet name="insertion" sheetId="1" r:id="rId2"/>
     <sheet name="selection" sheetId="3" r:id="rId3"/>
     <sheet name="quicksort" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="13">
   <si>
     <t>Sorting</t>
   </si>
@@ -566,11 +566,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -643,15 +650,131 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sorted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>bubble!$C$3:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>bubble!$F$3:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>839.19999999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3220</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12780</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>51180</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>205000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>820000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3285000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Inverse</c:v>
           </c:tx>
@@ -681,10 +804,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>insertion!$C$16:$C$28</c:f>
+              <c:f>bubble!$C$14:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
@@ -717,60 +840,48 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>524288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>insertion!$F$16:$F$28</c:f>
+              <c:f>bubble!$F$14:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.193</c:v>
+                  <c:v>3.7570000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33200000000000002</c:v>
+                  <c:v>15.952999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65300000000000002</c:v>
+                  <c:v>58.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3049999999999999</c:v>
+                  <c:v>222.20000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.601</c:v>
+                  <c:v>857.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1950000000000003</c:v>
+                  <c:v>3450</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.5</c:v>
+                  <c:v>13550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.7</c:v>
+                  <c:v>54090</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.599999999999994</c:v>
+                  <c:v>818000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>213.60000000000002</c:v>
+                  <c:v>3319000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>678.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>204970</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>81931000</c:v>
+                  <c:v>13237000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,16 +890,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Random</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -811,10 +920,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>insertion!$C$29:$C$41</c:f>
+              <c:f>bubble!$C$25:$C$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
@@ -847,188 +956,48 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>524288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>insertion!$F$29:$F$41</c:f>
+              <c:f>bubble!$F$25:$F$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19500000000000001</c:v>
+                  <c:v>3.6879999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.33799999999999997</c:v>
+                  <c:v>16.23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67699999999999994</c:v>
+                  <c:v>60.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.325</c:v>
+                  <c:v>223.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6179999999999999</c:v>
+                  <c:v>844.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2359999999999998</c:v>
+                  <c:v>3500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.299999999999999</c:v>
+                  <c:v>13840</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.6</c:v>
+                  <c:v>55440</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>58.2</c:v>
+                  <c:v>1544000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>148.19999999999999</c:v>
+                  <c:v>6332000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>419.9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>102370</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40866000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Sorted</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>insertion!$C$3:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>131072</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>262144</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>524288</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>insertion!$F$3:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>5.3999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0000000000000011E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.187</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.77399999999999991</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.403</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.9020000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.55</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>23.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45.1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>88.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>178.2</c:v>
+                  <c:v>25159000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1043,11 +1012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-354603072"/>
-        <c:axId val="-354604160"/>
+        <c:axId val="1475034368"/>
+        <c:axId val="1475032192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-354603072"/>
+        <c:axId val="1475034368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,16 +1073,14 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-354604160"/>
+        <c:crossAx val="1475032192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-354604160"/>
+        <c:axId val="1475032192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="90000000"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1168,7 +1135,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-354603072"/>
+        <c:crossAx val="1475034368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1263,15 +1230,273 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Inverse</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>insertion!$C$16:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>insertion!$F$16:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.65300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.601</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>213.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>678.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204970</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81931000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Random</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>insertion!$C$29:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>524288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>insertion!$F$29:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6179999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2359999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>148.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>419.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>102370</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40866000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Sorted</c:v>
           </c:tx>
@@ -1301,10 +1526,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>bubble!$C$3:$C$14</c:f>
+              <c:f>insertion!$C$3:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
@@ -1340,283 +1565,57 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>524288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>bubble!$F$3:$F$14</c:f>
+              <c:f>insertion!$F$3:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>4.077</c:v>
+                  <c:v>5.3999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.7</c:v>
+                  <c:v>9.0000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56</c:v>
+                  <c:v>0.187</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>215.7</c:v>
+                  <c:v>0.39800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>839.19999999999993</c:v>
+                  <c:v>0.77399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3220</c:v>
+                  <c:v>1.403</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12780</c:v>
+                  <c:v>2.9020000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51180</c:v>
+                  <c:v>5.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>205000</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>820000</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3285000</c:v>
+                  <c:v>45.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13381000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Inverse</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>bubble!$C$15:$C$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>131072</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>bubble!$F$15:$F$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3.7570000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15.952999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58.7</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>222.20000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>857.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3450</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13550</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>54090</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>818000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3319000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>13237000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Random</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>bubble!$C$26:$C$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>256</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4096</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8192</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32768</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>65536</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>131072</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>bubble!$F$26:$F$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>3.6879999999999997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.23</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>223.3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>844.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13840</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55440</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1544000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6332000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25159000</c:v>
+                  <c:v>88.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1631,11 +1630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-450183648"/>
-        <c:axId val="-450198336"/>
+        <c:axId val="1470243584"/>
+        <c:axId val="1470244128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-450183648"/>
+        <c:axId val="1470243584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,14 +1691,16 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-450198336"/>
+        <c:crossAx val="1470244128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-450198336"/>
+        <c:axId val="1470244128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="90000000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1754,7 +1755,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-450183648"/>
+        <c:crossAx val="1470243584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2229,11 +2230,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-451476752"/>
-        <c:axId val="-451464240"/>
+        <c:axId val="1475031104"/>
+        <c:axId val="1475027840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-451476752"/>
+        <c:axId val="1475031104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2290,12 +2291,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-451464240"/>
+        <c:crossAx val="1475027840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-451464240"/>
+        <c:axId val="1475027840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2352,7 +2353,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-451476752"/>
+        <c:crossAx val="1475031104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2845,11 +2846,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-486152112"/>
-        <c:axId val="-486152656"/>
+        <c:axId val="1475026752"/>
+        <c:axId val="1475033824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-486152112"/>
+        <c:axId val="1475026752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,12 +2907,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-486152656"/>
+        <c:crossAx val="1475033824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-486152656"/>
+        <c:axId val="1475033824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,7 +2969,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-486152112"/>
+        <c:crossAx val="1475026752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5278,19 +5279,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>723899</xdr:colOff>
+      <xdr:colOff>761999</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>752474</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5313,19 +5314,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
+      <xdr:colOff>723899</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>733424</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>752474</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5676,10 +5677,645 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>128</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4077</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="F3" s="1">
+        <f>(D3/E3)*1000</f>
+        <v>4.077</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>256</v>
+      </c>
+      <c r="D4" s="1">
+        <v>147</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F13" si="0">(D4/E4)*1000</f>
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>512</v>
+      </c>
+      <c r="D5" s="1">
+        <v>560</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2157</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>215.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2048</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8392</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>839.19999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4096</v>
+      </c>
+      <c r="D8" s="1">
+        <v>322</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>3220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1278</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>12780</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>16384</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5118</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>51180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>32768</v>
+      </c>
+      <c r="D11" s="1">
+        <v>205</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>205000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>65536</v>
+      </c>
+      <c r="D12" s="1">
+        <v>820</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>820000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>131072</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3285</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="0"/>
+        <v>3285000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>128</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3757</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="F14" s="1">
+        <f>(D14/E14)*1000</f>
+        <v>3.7570000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>256</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15953</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="F15" s="1">
+        <f>(D15/E15)*1000</f>
+        <v>15.952999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>512</v>
+      </c>
+      <c r="D16" s="1">
+        <v>587</v>
+      </c>
+      <c r="E16" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F16" s="1">
+        <f>(D16/E16)*1000</f>
+        <v>58.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2222</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F17" s="1">
+        <f>(D17/E17)*1000</f>
+        <v>222.20000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2048</v>
+      </c>
+      <c r="D18" s="1">
+        <v>8576</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F18" s="1">
+        <f>(D18/E18)*1000</f>
+        <v>857.6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4096</v>
+      </c>
+      <c r="D19" s="1">
+        <v>345</v>
+      </c>
+      <c r="E19" s="1">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1">
+        <f>(D19/E19)*1000</f>
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1355</v>
+      </c>
+      <c r="E20" s="1">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1">
+        <f>(D20/E20)*1000</f>
+        <v>13550</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1">
+        <v>16384</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5409</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100</v>
+      </c>
+      <c r="F21" s="1">
+        <f>(D21/E21)*1000</f>
+        <v>54090</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1">
+        <v>32768</v>
+      </c>
+      <c r="D22" s="1">
+        <v>818</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <f>(D22/E22)*1000</f>
+        <v>818000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>65536</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3319</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <f>(D23/E23)*1000</f>
+        <v>3319000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="1">
+        <v>131072</v>
+      </c>
+      <c r="D24" s="1">
+        <v>13237</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <f>(D24/E24)*1000</f>
+        <v>13237000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1">
+        <v>128</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3688</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="F25" s="1">
+        <f>(D25/E25)*1000</f>
+        <v>3.6879999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>256</v>
+      </c>
+      <c r="D26" s="1">
+        <v>16230</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="F26" s="1">
+        <f>(D26/E26)*1000</f>
+        <v>16.23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>512</v>
+      </c>
+      <c r="D27" s="1">
+        <v>602</v>
+      </c>
+      <c r="E27" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F27" s="1">
+        <f>(D27/E27)*1000</f>
+        <v>60.199999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2233</v>
+      </c>
+      <c r="E28" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F28" s="1">
+        <f>(D28/E28)*1000</f>
+        <v>223.3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2048</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8447</v>
+      </c>
+      <c r="E29" s="1">
+        <v>10000</v>
+      </c>
+      <c r="F29" s="1">
+        <f>(D29/E29)*1000</f>
+        <v>844.7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4096</v>
+      </c>
+      <c r="D30" s="1">
+        <v>350</v>
+      </c>
+      <c r="E30" s="1">
+        <v>100</v>
+      </c>
+      <c r="F30" s="1">
+        <f>(D30/E30)*1000</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="1">
+        <v>8192</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1384</v>
+      </c>
+      <c r="E31" s="1">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1">
+        <f>(D31/E31)*1000</f>
+        <v>13840</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
+        <v>16384</v>
+      </c>
+      <c r="D32" s="1">
+        <v>5544</v>
+      </c>
+      <c r="E32" s="1">
+        <v>100</v>
+      </c>
+      <c r="F32" s="1">
+        <f>(D32/E32)*1000</f>
+        <v>55440</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1">
+        <v>32768</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1544</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <f>(D33/E33)*1000</f>
+        <v>1544000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1">
+        <v>65536</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6332</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <f>(D34/E34)*1000</f>
+        <v>6332000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1">
+        <v>131072</v>
+      </c>
+      <c r="D35" s="1">
+        <v>25159</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <f>(D35/E35)*1000</f>
+        <v>25159000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6191,7 +6827,7 @@
         <v>1000000</v>
       </c>
       <c r="F29" s="1">
-        <f>(D29/E29) *1000</f>
+        <f t="shared" ref="F29:F41" si="1">(D29/E29) *1000</f>
         <v>0.19500000000000001</v>
       </c>
     </row>
@@ -6209,7 +6845,7 @@
         <v>1000000</v>
       </c>
       <c r="F30" s="1">
-        <f>(D30/E30) *1000</f>
+        <f t="shared" si="1"/>
         <v>0.33799999999999997</v>
       </c>
     </row>
@@ -6227,7 +6863,7 @@
         <v>1000000</v>
       </c>
       <c r="F31" s="1">
-        <f>(D31/E31) *1000</f>
+        <f t="shared" si="1"/>
         <v>0.67699999999999994</v>
       </c>
     </row>
@@ -6245,7 +6881,7 @@
         <v>1000000</v>
       </c>
       <c r="F32" s="1">
-        <f>(D32/E32) *1000</f>
+        <f t="shared" si="1"/>
         <v>1.325</v>
       </c>
     </row>
@@ -6263,7 +6899,7 @@
         <v>1000000</v>
       </c>
       <c r="F33" s="1">
-        <f>(D33/E33) *1000</f>
+        <f t="shared" si="1"/>
         <v>2.6179999999999999</v>
       </c>
     </row>
@@ -6281,7 +6917,7 @@
         <v>1000000</v>
       </c>
       <c r="F34" s="1">
-        <f>(D34/E34) *1000</f>
+        <f t="shared" si="1"/>
         <v>5.2359999999999998</v>
       </c>
     </row>
@@ -6299,7 +6935,7 @@
         <v>10000</v>
       </c>
       <c r="F35" s="1">
-        <f>(D35/E35) *1000</f>
+        <f t="shared" si="1"/>
         <v>11.299999999999999</v>
       </c>
     </row>
@@ -6317,7 +6953,7 @@
         <v>10000</v>
       </c>
       <c r="F36" s="1">
-        <f>(D36/E36) *1000</f>
+        <f t="shared" si="1"/>
         <v>24.6</v>
       </c>
     </row>
@@ -6335,7 +6971,7 @@
         <v>10000</v>
       </c>
       <c r="F37" s="1">
-        <f>(D37/E37) *1000</f>
+        <f t="shared" si="1"/>
         <v>58.2</v>
       </c>
     </row>
@@ -6353,7 +6989,7 @@
         <v>10000</v>
       </c>
       <c r="F38" s="1">
-        <f>(D38/E38) *1000</f>
+        <f t="shared" si="1"/>
         <v>148.19999999999999</v>
       </c>
     </row>
@@ -6371,7 +7007,7 @@
         <v>10000</v>
       </c>
       <c r="F39" s="1">
-        <f>(D39/E39) *1000</f>
+        <f t="shared" si="1"/>
         <v>419.9</v>
       </c>
     </row>
@@ -6389,7 +7025,7 @@
         <v>100</v>
       </c>
       <c r="F40" s="1">
-        <f>(D40/E40) *1000</f>
+        <f t="shared" si="1"/>
         <v>102370</v>
       </c>
     </row>
@@ -6407,7 +7043,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="1">
-        <f>(D41/E41) *1000</f>
+        <f t="shared" si="1"/>
         <v>40866000</v>
       </c>
     </row>
@@ -6418,664 +7054,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F36"/>
-  <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>128</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4077</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F3" s="1">
-        <f>(D3/E3)*1000</f>
-        <v>4.077</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>256</v>
-      </c>
-      <c r="D4" s="1">
-        <v>147</v>
-      </c>
-      <c r="E4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F36" si="0">(D4/E4)*1000</f>
-        <v>14.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>512</v>
-      </c>
-      <c r="D5" s="1">
-        <v>560</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1024</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2157</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>215.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2048</v>
-      </c>
-      <c r="D7" s="1">
-        <v>8392</v>
-      </c>
-      <c r="E7" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>839.19999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4096</v>
-      </c>
-      <c r="D8" s="1">
-        <v>322</v>
-      </c>
-      <c r="E8" s="1">
-        <v>100</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>3220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8192</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1278</v>
-      </c>
-      <c r="E9" s="1">
-        <v>100</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>12780</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1">
-        <v>16384</v>
-      </c>
-      <c r="D10" s="1">
-        <v>5118</v>
-      </c>
-      <c r="E10" s="1">
-        <v>100</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>51180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>32768</v>
-      </c>
-      <c r="D11" s="1">
-        <v>205</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>205000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1">
-        <v>65536</v>
-      </c>
-      <c r="D12" s="1">
-        <v>820</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>820000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1">
-        <v>131072</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3285</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>3285000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1">
-        <v>262144</v>
-      </c>
-      <c r="D14" s="1">
-        <v>13381</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>13381000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1">
-        <v>128</v>
-      </c>
-      <c r="D15" s="1">
-        <v>3757</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>3.7570000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1">
-        <v>256</v>
-      </c>
-      <c r="D16" s="1">
-        <v>15953</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>15.952999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1">
-        <v>512</v>
-      </c>
-      <c r="D17" s="1">
-        <v>587</v>
-      </c>
-      <c r="E17" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>58.7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1024</v>
-      </c>
-      <c r="D18" s="1">
-        <v>2222</v>
-      </c>
-      <c r="E18" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>222.20000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2048</v>
-      </c>
-      <c r="D19" s="1">
-        <v>8576</v>
-      </c>
-      <c r="E19" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>857.6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="1">
-        <v>4096</v>
-      </c>
-      <c r="D20" s="1">
-        <v>345</v>
-      </c>
-      <c r="E20" s="1">
-        <v>100</v>
-      </c>
-      <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>3450</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="1">
-        <v>8192</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1355</v>
-      </c>
-      <c r="E21" s="1">
-        <v>100</v>
-      </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>13550</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1">
-        <v>16384</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5409</v>
-      </c>
-      <c r="E22" s="1">
-        <v>100</v>
-      </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>54090</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1">
-        <v>32768</v>
-      </c>
-      <c r="D23" s="1">
-        <v>818</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>818000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1">
-        <v>65536</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3319</v>
-      </c>
-      <c r="E24" s="1">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>3319000</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="1">
-        <v>131072</v>
-      </c>
-      <c r="D25" s="1">
-        <v>13237</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>13237000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1">
-        <v>128</v>
-      </c>
-      <c r="D26" s="1">
-        <v>3688</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>3.6879999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1">
-        <v>256</v>
-      </c>
-      <c r="D27" s="1">
-        <v>16230</v>
-      </c>
-      <c r="E27" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>16.23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1">
-        <v>512</v>
-      </c>
-      <c r="D28" s="1">
-        <v>602</v>
-      </c>
-      <c r="E28" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F28" s="1">
-        <f t="shared" si="0"/>
-        <v>60.199999999999996</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1024</v>
-      </c>
-      <c r="D29" s="1">
-        <v>2233</v>
-      </c>
-      <c r="E29" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F29" s="1">
-        <f t="shared" si="0"/>
-        <v>223.3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1">
-        <v>2048</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8447</v>
-      </c>
-      <c r="E30" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="0"/>
-        <v>844.7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1">
-        <v>4096</v>
-      </c>
-      <c r="D31" s="1">
-        <v>350</v>
-      </c>
-      <c r="E31" s="1">
-        <v>100</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="0"/>
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1">
-        <v>8192</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1384</v>
-      </c>
-      <c r="E32" s="1">
-        <v>100</v>
-      </c>
-      <c r="F32" s="1">
-        <f t="shared" si="0"/>
-        <v>13840</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="1">
-        <v>16384</v>
-      </c>
-      <c r="D33" s="1">
-        <v>5544</v>
-      </c>
-      <c r="E33" s="1">
-        <v>100</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="0"/>
-        <v>55440</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="1">
-        <v>32768</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1544</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="0"/>
-        <v>1544000</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="1">
-        <v>65536</v>
-      </c>
-      <c r="D35" s="1">
-        <v>6332</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <f t="shared" si="0"/>
-        <v>6332000</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1">
-        <v>131072</v>
-      </c>
-      <c r="D36" s="1">
-        <v>25159</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1">
-        <f t="shared" si="0"/>
-        <v>25159000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B25" sqref="B25:E26"/>
     </sheetView>
   </sheetViews>
@@ -7553,7 +7536,7 @@
         <v>1000000</v>
       </c>
       <c r="F27" s="1">
-        <f>(D27/E27)*1000</f>
+        <f t="shared" ref="F27:F38" si="1">(D27/E27)*1000</f>
         <v>3.5350000000000001</v>
       </c>
     </row>
@@ -7571,7 +7554,7 @@
         <v>1000000</v>
       </c>
       <c r="F28" s="1">
-        <f>(D28/E28)*1000</f>
+        <f t="shared" si="1"/>
         <v>11.102</v>
       </c>
     </row>
@@ -7589,7 +7572,7 @@
         <v>10000</v>
       </c>
       <c r="F29" s="1">
-        <f>(D29/E29)*1000</f>
+        <f t="shared" si="1"/>
         <v>41.8</v>
       </c>
     </row>
@@ -7607,7 +7590,7 @@
         <v>10000</v>
       </c>
       <c r="F30" s="1">
-        <f>(D30/E30)*1000</f>
+        <f t="shared" si="1"/>
         <v>165.20000000000002</v>
       </c>
     </row>
@@ -7625,7 +7608,7 @@
         <v>10000</v>
       </c>
       <c r="F31" s="1">
-        <f>(D31/E31)*1000</f>
+        <f t="shared" si="1"/>
         <v>556.6</v>
       </c>
     </row>
@@ -7643,7 +7626,7 @@
         <v>100</v>
       </c>
       <c r="F32" s="1">
-        <f>(D32/E32)*1000</f>
+        <f t="shared" si="1"/>
         <v>2120</v>
       </c>
     </row>
@@ -7661,7 +7644,7 @@
         <v>100</v>
       </c>
       <c r="F33" s="1">
-        <f>(D33/E33)*1000</f>
+        <f t="shared" si="1"/>
         <v>8310</v>
       </c>
     </row>
@@ -7679,7 +7662,7 @@
         <v>100</v>
       </c>
       <c r="F34" s="1">
-        <f>(D34/E34)*1000</f>
+        <f t="shared" si="1"/>
         <v>33280</v>
       </c>
     </row>
@@ -7697,7 +7680,7 @@
         <v>100</v>
       </c>
       <c r="F35" s="1">
-        <f>(D35/E35)*1000</f>
+        <f t="shared" si="1"/>
         <v>133230</v>
       </c>
     </row>
@@ -7715,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1">
-        <f>(D36/E36)*1000</f>
+        <f t="shared" si="1"/>
         <v>542000</v>
       </c>
     </row>
@@ -7733,7 +7716,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1">
-        <f>(D37/E37)*1000</f>
+        <f t="shared" si="1"/>
         <v>2165000</v>
       </c>
     </row>
@@ -7751,7 +7734,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="1">
-        <f>(D38/E38)*1000</f>
+        <f t="shared" si="1"/>
         <v>8961000</v>
       </c>
     </row>
@@ -7763,10 +7746,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F41"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8499,6 +8482,96 @@
         <v>512000</v>
       </c>
     </row>
+    <row r="43" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C43" s="3"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C44" s="3"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="2:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C51" s="3"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C52" s="3"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C54" s="3"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C57" s="3"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="3:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="C58" s="3"/>
+      <c r="F58" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>